<commit_message>
Add Employee page also in progress
</commit_message>
<xml_diff>
--- a/OrangeHRM_Project/src/test/resources/TestData/Keywords.xlsx
+++ b/OrangeHRM_Project/src/test/resources/TestData/Keywords.xlsx
@@ -7,7 +7,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>login</t>
+  </si>
+  <si>
+    <t>validate</t>
   </si>
   <si>
     <t>logout</t>
@@ -414,8 +417,8 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -424,8 +427,9 @@
     <col min="2" max="2" width="18.33203" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.66406" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.66406" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.66406" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.66406" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.66406" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.66406" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.66406" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -442,9 +446,12 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -467,10 +474,13 @@
       <c r="F2" t="s">
         <v>9</v>
       </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -481,13 +491,16 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" t="s">
-        <v>9</v>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -498,13 +511,16 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" t="s">
-        <v>9</v>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -515,13 +531,16 @@
       <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" t="s">
-        <v>9</v>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -532,13 +551,16 @@
       <c r="D6" t="s">
         <v>7</v>
       </c>
-      <c r="F6" t="s">
-        <v>9</v>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -549,13 +571,16 @@
       <c r="D7" t="s">
         <v>7</v>
       </c>
-      <c r="F7" t="s">
-        <v>9</v>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -566,8 +591,11 @@
       <c r="D8" t="s">
         <v>7</v>
       </c>
-      <c r="F8" t="s">
-        <v>9</v>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -577,7 +605,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -594,7 +622,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="15.6">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -606,7 +634,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -620,7 +648,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -629,21 +657,21 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -651,17 +679,16 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="E3"/>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -669,17 +696,16 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="E4"/>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -687,17 +713,16 @@
       <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="E5"/>
       <c r="G5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -705,17 +730,16 @@
       <c r="D6" t="s">
         <v>7</v>
       </c>
-      <c r="E6"/>
       <c r="G6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -723,17 +747,16 @@
       <c r="D7" t="s">
         <v>7</v>
       </c>
-      <c r="E7"/>
       <c r="G7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -741,9 +764,8 @@
       <c r="D8" t="s">
         <v>7</v>
       </c>
-      <c r="E8"/>
       <c r="G8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Employee list is progress
</commit_message>
<xml_diff>
--- a/OrangeHRM_Project/src/test/resources/TestData/Keywords.xlsx
+++ b/OrangeHRM_Project/src/test/resources/TestData/Keywords.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationTesting\OrangeHRM_Project\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationTesting\OrangeHRM_Project\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
     <sheet name="AddEmployeePage" sheetId="2" r:id="rId2"/>
+    <sheet name="EmployeeListPage" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr/>
 </workbook>
@@ -20,7 +21,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
-    <t>testCaseNo</t>
+    <t>TestCaseNo</t>
   </si>
   <si>
     <t>utils.BrowserUtils</t>
@@ -71,13 +72,16 @@
     <t>testCase07</t>
   </si>
   <si>
-    <t>TestCaseNo</t>
+    <t>pages.DashboardPage</t>
   </si>
   <si>
     <t>pages.AddEmployeePage</t>
   </si>
   <si>
     <t>openBrowser</t>
+  </si>
+  <si>
+    <t>performPIM</t>
   </si>
   <si>
     <t>performSave</t>
@@ -87,7 +91,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -97,6 +101,12 @@
     <font>
       <b/>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -115,9 +125,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,41 +428,41 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.44141" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.88672" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.33203" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.66406" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.66406" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.66406" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.66406" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.66406" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44141" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.44141" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
+    <row r="1" s="1" customFormat="1" ht="15.6">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -605,8 +616,8 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -615,14 +626,15 @@
     <col min="2" max="2" width="17.44141" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.44141" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.44141" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.55469" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.44141" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="15.6">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -634,12 +646,15 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -660,9 +675,12 @@
         <v>20</v>
       </c>
       <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -679,7 +697,8 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" t="s">
+      <c r="E3"/>
+      <c r="H3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -696,7 +715,8 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" t="s">
+      <c r="E4"/>
+      <c r="H4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -713,7 +733,8 @@
       <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="G5" t="s">
+      <c r="E5"/>
+      <c r="H5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -730,7 +751,8 @@
       <c r="D6" t="s">
         <v>7</v>
       </c>
-      <c r="G6" t="s">
+      <c r="E6"/>
+      <c r="H6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -747,7 +769,8 @@
       <c r="D7" t="s">
         <v>7</v>
       </c>
-      <c r="G7" t="s">
+      <c r="E7"/>
+      <c r="H7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -764,8 +787,147 @@
       <c r="D8" t="s">
         <v>7</v>
       </c>
-      <c r="G8" t="s">
-        <v>10</v>
+      <c r="E8"/>
+      <c r="H8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="11.88672" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44141" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44141" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.77734" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>